<commit_message>
Fixed Planned constraint bug, added turbines to data
</commit_message>
<xml_diff>
--- a/Code/Overlap/SolCheck.xlsx
+++ b/Code/Overlap/SolCheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAE0B79-5E7F-4E59-802F-261FCF7CDB27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D64CED-686B-4BEE-8B13-5CD2338B75AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1216E67F-FE2E-4197-BF88-EB74DB65ED3B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>Availability</t>
   </si>
@@ -258,21 +258,21 @@
   <dxfs count="4">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2986,8 +2986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A6C30D-2564-44ED-B130-7E857DB19B52}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,13 +2996,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
+      <c r="A1" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B1">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+        <f>SUM(D9:D20)+SUM(K24:K35)+SUM(G39:G50)</f>
+        <v>1835800</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E1">
@@ -3010,13 +3011,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2">
-        <v>70</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="A2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E2">
@@ -3024,13 +3020,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>720</v>
-      </c>
-      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E3">
@@ -3038,7 +3034,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>70</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>50</v>
       </c>
       <c r="E4">
@@ -3046,7 +3048,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>720</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E5">
@@ -3078,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f>(B9+C9)*$B$1*$B$2</f>
+        <f>(B9+C9)*$B$3*$B$4</f>
         <v>0</v>
       </c>
     </row>
@@ -3093,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10:D20" si="0">(B10+C10)*$B$1*$B$2</f>
+        <f>(B10+C10)*$B$3*$B$4</f>
         <v>0</v>
       </c>
     </row>
@@ -3108,7 +3116,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f>(B11+C11)*$B$3*$B$4</f>
         <v>0</v>
       </c>
     </row>
@@ -3123,7 +3131,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f>(B12+C12)*$B$3*$B$4</f>
         <v>0</v>
       </c>
     </row>
@@ -3138,7 +3146,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f>(B13+C13)*$B$3*$B$4</f>
         <v>0</v>
       </c>
     </row>
@@ -3153,7 +3161,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f>(B14+C14)*$B$3*$B$4</f>
         <v>0</v>
       </c>
     </row>
@@ -3162,14 +3170,14 @@
         <v>6</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>(B15+C15)*$B$3*$B$4</f>
+        <v>4550</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3183,7 +3191,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f>(B16+C16)*$B$3*$B$4</f>
         <v>0</v>
       </c>
     </row>
@@ -3192,14 +3200,14 @@
         <v>8</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>(B17+C17)*$B$3*$B$4</f>
+        <v>2450</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3213,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f>(B18+C18)*$B$3*$B$4</f>
         <v>0</v>
       </c>
     </row>
@@ -3228,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f>(B19+C19)*$B$3*$B$4</f>
         <v>0</v>
       </c>
     </row>
@@ -3243,7 +3251,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f>(B20+C20)*$B$3*$B$4</f>
         <v>0</v>
       </c>
     </row>
@@ -3309,11 +3317,11 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <f>SUM(B$24:B24,E$24:E24)*$B$2*$B$3</f>
+        <f>SUM(B$24:B24,E$24:E24)*$B$4*$B$5</f>
         <v>0</v>
       </c>
       <c r="J24">
-        <f>SUM(C$24:C24,F$24:F24)*$B$2*$B$3</f>
+        <f>SUM(C$24:C24,F$24:F24)*$B$4*$B$5</f>
         <v>0</v>
       </c>
       <c r="K24">
@@ -3346,15 +3354,15 @@
         <v>2</v>
       </c>
       <c r="I25">
-        <f>SUM(B$24:B25,E$24:E25)*$B$2*$B$3</f>
+        <f>SUM(B$24:B25,E$24:E25)*$B$4*$B$5</f>
         <v>100800</v>
       </c>
       <c r="J25">
-        <f>SUM(C$24:C25,F$24:F25)*$B$2*$B$3</f>
+        <f>SUM(C$24:C25,F$24:F25)*$B$4*$B$5</f>
         <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:K35" si="1">I25-J25</f>
+        <f t="shared" ref="K25:K35" si="0">I25-J25</f>
         <v>100800</v>
       </c>
     </row>
@@ -3369,7 +3377,7 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:D35" si="2">B26-C26+D25</f>
+        <f t="shared" ref="D26:D35" si="1">B26-C26+D25</f>
         <v>0</v>
       </c>
       <c r="E26">
@@ -3379,19 +3387,19 @@
         <v>2</v>
       </c>
       <c r="G26">
-        <f t="shared" ref="G26:G35" si="3">E26-F26+G25</f>
+        <f t="shared" ref="G26:G35" si="2">E26-F26+G25</f>
         <v>2</v>
       </c>
       <c r="I26">
-        <f>SUM(B$24:B26,E$24:E26)*$B$2*$B$3</f>
+        <f>SUM(B$24:B26,E$24:E26)*$B$4*$B$5</f>
         <v>201600</v>
       </c>
       <c r="J26">
-        <f>SUM(C$24:C26,F$24:F26)*$B$2*$B$3</f>
+        <f>SUM(C$24:C26,F$24:F26)*$B$4*$B$5</f>
         <v>100800</v>
       </c>
       <c r="K26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>100800</v>
       </c>
     </row>
@@ -3406,29 +3414,29 @@
         <v>0</v>
       </c>
       <c r="D27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="I27">
-        <f>SUM(B$24:B27,E$24:E27)*$B$2*$B$3</f>
+        <f>SUM(B$24:B27,E$24:E27)*$B$4*$B$5</f>
         <v>201600</v>
       </c>
       <c r="J27">
-        <f>SUM(C$24:C27,F$24:F27)*$B$2*$B$3</f>
+        <f>SUM(C$24:C27,F$24:F27)*$B$4*$B$5</f>
         <v>201600</v>
       </c>
       <c r="K27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3443,29 +3451,29 @@
         <v>0</v>
       </c>
       <c r="D28">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I28">
-        <f>SUM(B$24:B28,E$24:E28)*$B$2*$B$3</f>
+        <f>SUM(B$24:B28,E$24:E28)*$B$4*$B$5</f>
         <v>302400</v>
       </c>
       <c r="J28">
-        <f>SUM(C$24:C28,F$24:F28)*$B$2*$B$3</f>
+        <f>SUM(C$24:C28,F$24:F28)*$B$4*$B$5</f>
         <v>201600</v>
       </c>
       <c r="K28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>100800</v>
       </c>
     </row>
@@ -3480,29 +3488,29 @@
         <v>2</v>
       </c>
       <c r="D29">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I29">
-        <f>SUM(B$24:B29,E$24:E29)*$B$2*$B$3</f>
+        <f>SUM(B$24:B29,E$24:E29)*$B$4*$B$5</f>
         <v>453600</v>
       </c>
       <c r="J29">
-        <f>SUM(C$24:C29,F$24:F29)*$B$2*$B$3</f>
+        <f>SUM(C$24:C29,F$24:F29)*$B$4*$B$5</f>
         <v>302400</v>
       </c>
       <c r="K29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>151200</v>
       </c>
     </row>
@@ -3517,29 +3525,29 @@
         <v>3</v>
       </c>
       <c r="D30">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I30">
-        <f>SUM(B$24:B30,E$24:E30)*$B$2*$B$3</f>
+        <f>SUM(B$24:B30,E$24:E30)*$B$4*$B$5</f>
         <v>655200</v>
       </c>
       <c r="J30">
-        <f>SUM(C$24:C30,F$24:F30)*$B$2*$B$3</f>
+        <f>SUM(C$24:C30,F$24:F30)*$B$4*$B$5</f>
         <v>453600</v>
       </c>
       <c r="K30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>201600</v>
       </c>
     </row>
@@ -3554,29 +3562,29 @@
         <v>4</v>
       </c>
       <c r="D31">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I31">
-        <f>SUM(B$24:B31,E$24:E31)*$B$2*$B$3</f>
+        <f>SUM(B$24:B31,E$24:E31)*$B$4*$B$5</f>
         <v>907200</v>
       </c>
       <c r="J31">
-        <f>SUM(C$24:C31,F$24:F31)*$B$2*$B$3</f>
+        <f>SUM(C$24:C31,F$24:F31)*$B$4*$B$5</f>
         <v>655200</v>
       </c>
       <c r="K31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>252000</v>
       </c>
     </row>
@@ -3591,7 +3599,7 @@
         <v>5</v>
       </c>
       <c r="D32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E32">
@@ -3601,19 +3609,19 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I32">
-        <f>SUM(B$24:B32,E$24:E32)*$B$2*$B$3</f>
+        <f>SUM(B$24:B32,E$24:E32)*$B$4*$B$5</f>
         <v>1159200</v>
       </c>
       <c r="J32">
-        <f>SUM(C$24:C32,F$24:F32)*$B$2*$B$3</f>
+        <f>SUM(C$24:C32,F$24:F32)*$B$4*$B$5</f>
         <v>907200</v>
       </c>
       <c r="K32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>252000</v>
       </c>
     </row>
@@ -3628,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E33">
@@ -3638,19 +3646,19 @@
         <v>5</v>
       </c>
       <c r="G33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I33">
-        <f>SUM(B$24:B33,E$24:E33)*$B$2*$B$3</f>
+        <f>SUM(B$24:B33,E$24:E33)*$B$4*$B$5</f>
         <v>1310400</v>
       </c>
       <c r="J33">
-        <f>SUM(C$24:C33,F$24:F33)*$B$2*$B$3</f>
+        <f>SUM(C$24:C33,F$24:F33)*$B$4*$B$5</f>
         <v>1159200</v>
       </c>
       <c r="K33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>151200</v>
       </c>
     </row>
@@ -3665,7 +3673,7 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E34">
@@ -3675,19 +3683,19 @@
         <v>3</v>
       </c>
       <c r="G34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I34">
-        <f>SUM(B$24:B34,E$24:E34)*$B$2*$B$3</f>
+        <f>SUM(B$24:B34,E$24:E34)*$B$4*$B$5</f>
         <v>1713600</v>
       </c>
       <c r="J34">
-        <f>SUM(C$24:C34,F$24:F34)*$B$2*$B$3</f>
+        <f>SUM(C$24:C34,F$24:F34)*$B$4*$B$5</f>
         <v>1310400</v>
       </c>
       <c r="K34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>403200</v>
       </c>
     </row>
@@ -3702,29 +3710,29 @@
         <v>8</v>
       </c>
       <c r="D35">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I35">
-        <f>SUM(B$24:B35,E$24:E35)*$B$2*$B$3</f>
+        <f>SUM(B$24:B35,E$24:E35)*$B$4*$B$5</f>
         <v>1814400</v>
       </c>
       <c r="J35">
-        <f>SUM(C$24:C35,F$24:F35)*$B$2*$B$3</f>
+        <f>SUM(C$24:C35,F$24:F35)*$B$4*$B$5</f>
         <v>1713600</v>
       </c>
       <c r="K35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>100800</v>
       </c>
     </row>
@@ -3764,13 +3772,17 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <f>B39*$E$1+C39</f>
+        <f t="shared" ref="D39:D50" si="3">B39*$E$1+C39</f>
         <v>0</v>
       </c>
       <c r="E39">
         <f>(B9+C9)*$E$2+C24*$E$4+F24*$E$5</f>
         <v>0</v>
       </c>
+      <c r="G39">
+        <f>B39*$E$3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -3783,13 +3795,17 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <f>B40*$E$1+C40</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E40">
         <f t="shared" ref="E40:E50" si="4">(B10+C10)*$E$2+C25*$E$4+F25*$E$5</f>
         <v>0</v>
       </c>
+      <c r="G40">
+        <f t="shared" ref="G40:G50" si="5">B40*$E$3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -3802,13 +3818,17 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <f>B41*$E$1+C41</f>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="E41">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
+      <c r="G41">
+        <f t="shared" si="5"/>
+        <v>1800</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -3821,13 +3841,17 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <f>B42*$E$1+C42</f>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="E42">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
+      <c r="G42">
+        <f t="shared" si="5"/>
+        <v>1800</v>
+      </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -3840,11 +3864,15 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <f>B43*$E$1+C43</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E43">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3859,13 +3887,17 @@
         <v>0</v>
       </c>
       <c r="D44">
-        <f>B44*$E$1+C44</f>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="E44">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
+      <c r="G44">
+        <f t="shared" si="5"/>
+        <v>1800</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -3878,12 +3910,16 @@
         <v>80</v>
       </c>
       <c r="D45">
-        <f>B45*$E$1+C45</f>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="E45">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>77</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -3897,13 +3933,17 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <f>B46*$E$1+C46</f>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="E46">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
+      <c r="G46">
+        <f t="shared" si="5"/>
+        <v>1800</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -3916,12 +3956,16 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <f>B47*$E$1+C47</f>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="E47">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>55</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="5"/>
+        <v>1800</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -3935,15 +3979,19 @@
         <v>0</v>
       </c>
       <c r="D48">
-        <f>B48*$E$1+C48</f>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="E48">
         <f t="shared" si="4"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <f t="shared" si="5"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>10</v>
       </c>
@@ -3954,15 +4002,19 @@
         <v>0</v>
       </c>
       <c r="D49">
-        <f>B49*$E$1+C49</f>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="E49">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <f t="shared" si="5"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>11</v>
       </c>
@@ -3973,12 +4025,16 @@
         <v>0</v>
       </c>
       <c r="D50">
-        <f>B50*$E$1+C50</f>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="E50">
         <f t="shared" si="4"/>
         <v>32</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="5"/>
+        <v>1800</v>
       </c>
     </row>
   </sheetData>
@@ -3991,10 +4047,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39:E50">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
       <formula>$D39</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>$D39</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>